<commit_message>
Hide added back button
</commit_message>
<xml_diff>
--- a/Submittals Export.xlsx
+++ b/Submittals Export.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Submittal" sheetId="2" r:id="Rdce22e1b6be54ae8"/>
+    <x:sheet name="Submittal" sheetId="2" r:id="R4ff3ce93cf6944af"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -6154,7 +6154,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="Re18c0d4630f54ee8" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="R7bac22c44d214274" cstate="print"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -48647,6 +48647,6 @@
       </x:c>
     </x:row>
   </x:sheetData>
-  <x:drawing r:id="R653e8ccc375349a1"/>
+  <x:drawing r:id="Rd9b7aadf65d94811"/>
 </x:worksheet>
 </file>
</xml_diff>